<commit_message>
edited pixel_heights.xlsx with the correct pixels heights. The previous version is saved as pixel_heights_old.xlsx
</commit_message>
<xml_diff>
--- a/CAD/pixel_heights.xlsx
+++ b/CAD/pixel_heights.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_57D4C4CE9EF4EE24F2142AAACE09D15AE3DBADB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E134CFD-54CC-4CDC-9FB7-0C934621A478}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="28680" yWindow="750" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,18 +457,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -493,12 +487,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -778,1165 +769,1165 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
-        <v>2.3211133664068799</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="1">
+        <v>3.2718805875289698</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>1.5889937563998699</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="1">
+        <v>2.5397609775219498</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>4.6400578978239304</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="1">
+        <v>5.5908251189460199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <v>4.1766649408313903</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="1">
+        <v>5.12743216195347</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>3.1841350410047302</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="1">
+        <v>4.1349022621268201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <v>2.9880831144456899</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="1">
+        <v>3.9388503355677802</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <v>2.25248473138977</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="1">
+        <v>3.2032519525118501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
-        <v>2.3238989262091998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="1">
+        <v>3.2746661473312901</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
-        <v>1.86777205688921</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="1">
+        <v>2.8185392780113001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
-        <v>2.2090278277522799</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="1">
+        <v>3.1597950488743698</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
-        <v>2.6868086772960198</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="1">
+        <v>4.4950758984181096</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
-        <v>2.3990482819228598</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="1">
+        <v>3.3498155030449399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
-        <v>1.42095714579285</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="1">
+        <v>2.3717243669149402</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
-        <v>0.68508873093704903</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="1">
+        <v>2.49335595205913</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
-        <v>3.7328409656410799</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="1">
+        <v>4.68360818676316</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
-        <v>2.6035786995934602</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="1">
+        <v>3.5543459207155501</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
-        <v>2.2712870016533202</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="1">
+        <v>3.2220542227753999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
-        <v>1.3996637411035</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="1">
+        <v>2.3504309622255901</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
-        <v>1.33496609158931</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="1">
+        <v>2.2857333127113901</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
-        <v>0.74234207017582499</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="1">
+        <v>5.9806092912979096</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
-        <v>0.94645081721513402</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="1">
+        <v>6.1847180383372198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
-        <v>1.28623632142704</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="1">
+        <v>2.2370035425491301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
-        <v>0.85953336552083504</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" s="1">
+        <v>6.0978005866429204</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="2">
-        <v>1.4746912659586999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" s="1">
+        <v>2.42545848708078</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
-        <v>0.69469914229088603</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" s="1">
+        <v>5.9329663634129703</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="2">
-        <v>2.52829764138865</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26" s="1">
+        <v>2.6215648625107399</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="2">
-        <v>3.00085809714618</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" s="1">
+        <v>3.9516253182682699</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="2">
-        <v>1.8691736500954701</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" s="1">
+        <v>2.8199408712175602</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="2">
-        <v>1.53466896520148</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29" s="1">
+        <v>2.4854361863235699</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="2">
-        <v>0.66099743092297003</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" s="1">
+        <v>5.8992646520450496</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="2">
-        <v>0.59439189672637305</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" s="1">
+        <v>5.8326591178484604</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" s="1">
+        <v>5.2382672211220802</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="2">
-        <v>0.202507676793828</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" s="1">
+        <v>5.4407748979159098</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="2">
-        <v>0.54091533665480096</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" s="1">
+        <v>2.3491825577768801</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="2">
-        <v>4.4006450801192001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" s="1">
+        <v>5.3514123012412904</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="2">
-        <v>0.72766392838453298</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" s="1">
+        <v>5.9659311495066198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="2">
-        <v>2.71884094594451</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" s="1">
+        <v>5.3846081670665997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="2">
-        <v>3.6926447104351001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" s="1">
+        <v>2.9284119315571902</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="2">
-        <v>5.0206609814554604</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39" s="1">
+        <v>3.3989282025775398</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="2">
-        <v>1.31462568715407</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" s="1">
+        <v>2.2653929082761599</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="2">
-        <v>3.5509150644162601</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" s="1">
+        <v>6.2166822855383401</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="2">
-        <v>4.3906464852865801</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" s="1">
+        <v>5.3414137064086598</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="2">
-        <v>2.6075325473537001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43" s="1">
+        <v>5.2732997684757796</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="2">
-        <v>3.7267194475243</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44" s="1">
+        <v>4.6774866686463898</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="2">
-        <v>2.2129131625049698</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45" s="1">
+        <v>4.87868038362706</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="2">
-        <v>3.36173152988408</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" s="1">
+        <v>4.3124987510061601</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="2">
-        <v>3.8364438427540901</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47" s="1">
+        <v>4.78721106387618</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="2">
-        <v>3.9206065553862901</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" s="1">
+        <v>4.8713737765083804</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="2">
-        <v>4.06649146253101</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49" s="1">
+        <v>5.0172586836531003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="2">
-        <v>3.3237559043885399</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50" s="1">
+        <v>3.4170231255106298</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="2">
-        <v>6.3653970506180997</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51" s="1">
+        <v>3.0286642717401899</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="2">
-        <v>5.2306109484433803</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52" s="1">
+        <v>6.1813781695654697</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="2">
-        <v>4.8932399544684397</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" s="1">
+        <v>5.8440071755905301</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="2">
-        <v>4.0168760593630601</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54" s="1">
+        <v>4.9676432804851496</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="2">
-        <v>3.9477173012027902</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55" s="1">
+        <v>4.8984845223248703</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="2">
-        <v>3.3509082742315202</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B56" s="1">
+        <v>4.30167549535361</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="2">
-        <v>3.5511682165398399</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57" s="1">
+        <v>4.5019354376619303</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="2">
-        <v>2.9841446635333799</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B58" s="1">
+        <v>3.9349118846554698</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="2">
-        <v>3.45815406384239</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B59" s="1">
+        <v>4.4089212849644701</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="2">
-        <v>3.5418175971962498</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B60" s="1">
+        <v>4.4925848183183401</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="2">
-        <v>3.8822768904538201</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B61" s="1">
+        <v>4.8330441115758997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="2">
-        <v>3.1387688196846102</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B62" s="1">
+        <v>3.2320360408066899</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="2">
-        <v>6.1797186484775102</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B63" s="1">
+        <v>2.8429858695996</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="2">
-        <v>5.0443019392504196</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B64" s="1">
+        <v>5.9950691603725001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="2">
-        <v>4.7063436070788702</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B65" s="1">
+        <v>5.6571108282009499</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="2">
-        <v>3.8294225178541899</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B66" s="1">
+        <v>4.7801897389762704</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="2">
-        <v>3.7597290899918301</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B67" s="1">
+        <v>4.7104963111139204</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="2">
-        <v>3.1624069029519202</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B68" s="1">
+        <v>4.1131741240740096</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B69" s="2">
-        <v>3.3621817788181101</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B69" s="1">
+        <v>4.3129489999402004</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="2">
-        <v>2.7947162716406999</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B70" s="1">
+        <v>3.74548349276278</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="2">
-        <v>3.2683508512719501</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B71" s="1">
+        <v>4.21911807239404</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="2">
-        <v>3.3517398349427299</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B72" s="1">
+        <v>4.30250705606481</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B73" s="2">
-        <v>3.8822768904538201</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B73" s="1">
+        <v>4.8330441115758997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B74" s="2">
-        <v>3.1387688196846102</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B74" s="1">
+        <v>3.2320360408066899</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B75" s="2">
-        <v>6.1797186484775102</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B75" s="1">
+        <v>2.8429858695996</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B76" s="2">
-        <v>5.0443019392504196</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B76" s="1">
+        <v>5.9950691603725001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B77" s="2">
-        <v>4.7063436070788702</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B77" s="1">
+        <v>5.6571108282009499</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B78" s="2">
-        <v>3.8294225178541899</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B78" s="1">
+        <v>4.7801897389762704</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B79" s="2">
-        <v>3.7597290899918301</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B79" s="1">
+        <v>4.7104963111139204</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B80" s="2">
-        <v>3.1624069029519202</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B80" s="1">
+        <v>4.1131741240740096</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B81" s="2">
-        <v>3.3621817788181101</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B81" s="1">
+        <v>4.3129489999402004</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B82" s="2">
-        <v>2.7947162716406999</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B82" s="1">
+        <v>3.74548349276278</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B83" s="2">
-        <v>3.2683508512719501</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B83" s="1">
+        <v>4.21911807239404</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B84" s="2">
-        <v>3.3517398349427299</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B84" s="1">
+        <v>4.30250705606481</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B85" s="2">
-        <v>4.06649146253101</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B85" s="1">
+        <v>5.0172586836531003</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B86" s="2">
-        <v>3.3237559043885399</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B86" s="1">
+        <v>3.4170231255106298</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B87" s="2">
-        <v>6.3653970506180997</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B87" s="1">
+        <v>3.0286642717401899</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B88" s="2">
-        <v>5.2306109484433803</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B88" s="1">
+        <v>6.1813781695654697</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B89" s="2">
-        <v>4.8932399544684397</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B89" s="1">
+        <v>5.8440071755905301</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B90" s="2">
-        <v>4.0168760593630601</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B90" s="1">
+        <v>4.9676432804851496</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B91" s="2">
-        <v>3.9477173012027902</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B91" s="1">
+        <v>4.8984845223248703</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B92" s="2">
-        <v>3.3509082742315202</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B92" s="1">
+        <v>4.30167549535361</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B93" s="2">
-        <v>3.5511682165398399</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B93" s="1">
+        <v>4.5019354376619303</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B94" s="2">
-        <v>2.9841446635333799</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B94" s="1">
+        <v>3.9349118846554698</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B95" s="2">
-        <v>3.45815406384239</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B95" s="1">
+        <v>4.4089212849644701</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B96" s="2">
-        <v>3.5418175971962498</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B96" s="1">
+        <v>4.4925848183183401</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B97" s="2">
-        <v>2.71884094594451</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B97" s="1">
+        <v>5.3846081670665997</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B98" s="2">
-        <v>3.6926447104351001</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B98" s="1">
+        <v>2.9284119315571902</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B99" s="2">
-        <v>5.0206609814554604</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B99" s="1">
+        <v>3.3989282025775398</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B100" s="2">
-        <v>1.31462568715407</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B100" s="1">
+        <v>2.2653929082761599</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B101" s="2">
-        <v>3.5509150644162601</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B101" s="1">
+        <v>6.2166822855383401</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B102" s="2">
-        <v>4.3906464852865801</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B102" s="1">
+        <v>5.3414137064086598</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B103" s="2">
-        <v>2.6075325473537001</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B103" s="1">
+        <v>5.2732997684757796</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B104" s="2">
-        <v>3.7267194475243</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B104" s="1">
+        <v>4.6774866686463898</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B105" s="2">
-        <v>2.2129131625049698</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B105" s="1">
+        <v>4.87868038362706</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B106" s="2">
-        <v>3.36173152988408</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B106" s="1">
+        <v>4.3124987510061601</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B107" s="2">
-        <v>3.8364438427540901</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B107" s="1">
+        <v>4.78721106387618</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B108" s="2">
-        <v>3.9206065553862901</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B108" s="1">
+        <v>4.8713737765083804</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B109" s="2">
-        <v>0.69469914229088603</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B109" s="1">
+        <v>5.9329663634129703</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B110" s="2">
-        <v>2.52829764138865</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B110" s="1">
+        <v>2.6215648625107399</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B111" s="2">
-        <v>3.00085809714618</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B111" s="1">
+        <v>3.9516253182682699</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B112" s="2">
-        <v>1.8691736500954701</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B112" s="1">
+        <v>2.8199408712175602</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B113" s="2">
-        <v>1.53466896520148</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B113" s="1">
+        <v>2.4854361863235699</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B114" s="2">
-        <v>0.66099743092297003</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B114" s="1">
+        <v>5.8992646520450496</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B115" s="2">
-        <v>0.59439189672637305</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B115" s="1">
+        <v>5.8326591178484604</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B116" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B116" s="1">
+        <v>5.2382672211220802</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B117" s="2">
-        <v>0.202507676793828</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B117" s="1">
+        <v>5.4407748979159098</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B118" s="2">
-        <v>3.92498911544061</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B118" s="1">
+        <v>4.8757563365627004</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B119" s="2">
-        <v>4.4006450801192001</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B119" s="1">
+        <v>5.3514123012412904</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B120" s="2">
-        <v>4.4854387030780298</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B120" s="1">
+        <v>5.4362059242001104</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B121" s="2">
-        <v>1.42095714579285</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B121" s="1">
+        <v>2.3717243669149402</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B122" s="2">
-        <v>0.68508873093704903</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B122" s="1">
+        <v>2.49335595205913</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B123" s="2">
-        <v>3.7328409656410799</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B123" s="1">
+        <v>4.68360818676316</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B124" s="2">
-        <v>2.6035786995934602</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B124" s="1">
+        <v>3.5543459207155501</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B125" s="2">
-        <v>2.2712870016533202</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B125" s="1">
+        <v>3.2220542227753999</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B126" s="2">
-        <v>1.3996637411035</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B126" s="1">
+        <v>2.3504309622255901</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B127" s="2">
-        <v>1.33496609158931</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B127" s="1">
+        <v>2.2857333127113901</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B128" s="2">
-        <v>0.74234207017582499</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B128" s="1">
+        <v>5.9806092912979096</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B129" s="2">
-        <v>0.94645081721513402</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B129" s="1">
+        <v>6.1847180383372198</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B130" s="2">
-        <v>2.0978101002128602</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B130" s="1">
+        <v>5.6210773213349396</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B131" s="2">
-        <v>0.85953336552083504</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B131" s="1">
+        <v>6.0978005866429204</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B132" s="2">
-        <v>5.2324660406521897</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B132" s="1">
+        <v>6.18323326177428</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B133" s="2">
-        <v>2.3211133664068799</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B133" s="1">
+        <v>3.2718805875289698</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B134" s="2">
-        <v>1.5889937563998699</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B134" s="1">
+        <v>2.5397609775219498</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B135" s="2">
-        <v>4.6400578978239304</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B135" s="1">
+        <v>5.5908251189460199</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B136" s="2">
-        <v>3.5137535068511001</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B136" s="1">
+        <v>4.4645207279731904</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B137" s="2">
-        <v>3.1841350410047302</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B137" s="1">
+        <v>4.1349022621268201</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B138" s="2">
-        <v>2.3149508465011901</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B138" s="1">
+        <v>3.26571806762328</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B139" s="2">
-        <v>2.25248473138977</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B139" s="1">
+        <v>3.2032519525118501</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B140" s="2">
-        <v>1.6618831778937599</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B140" s="1">
+        <v>2.6126503990158501</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B141" s="2">
-        <v>1.86777205688921</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B141" s="1">
+        <v>2.8185392780113001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B142" s="2">
-        <v>2.2090278277522799</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B142" s="1">
+        <v>3.1597950488743698</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B143" s="2">
-        <v>1.7833824560818301</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B143" s="1">
+        <v>2.73414967720392</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B144" s="2">
-        <v>2.3990482819228598</v>
+      <c r="B144" s="1">
+        <v>3.3498155030449399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>